<commit_message>
Separate tool for conversion of initial files
</commit_message>
<xml_diff>
--- a/Data/TDA_2_10_4.xlsx
+++ b/Data/TDA_2_10_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Modern\Desktop\Python\MTT assay multi\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5244CB-AC6D-48B7-87C1-7998BDDE6D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8891B83C-9835-4820-B71B-8CFE50ADA882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8391F9A9-44C2-405E-8E61-514D95C52142}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>1 mg/ml</t>
   </si>
@@ -54,7 +54,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,14 +89,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -400,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63E2702-D94C-41EA-8D69-209E054E43FF}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.63336000000000003</v>
       </c>
@@ -436,7 +447,7 @@
         <v>1.0646666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.62048999999999987</v>
       </c>
@@ -449,8 +460,20 @@
       <c r="D3">
         <v>0.92266666666666663</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.44499</v>
       </c>
@@ -463,8 +486,24 @@
       <c r="D4">
         <v>0.8686666666666667</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <f>AVERAGE(A2:A22)</f>
+        <v>0.81872142857142849</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:L4" si="0">AVERAGE(B2:B22)</f>
+        <v>0.83749714285714294</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>0.87237428571428577</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0.84442857142857142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.78077999999999992</v>
       </c>
@@ -477,8 +516,24 @@
       <c r="D5">
         <v>0.65066666666666662</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <f>_xlfn.STDEV.S(A2:A22)</f>
+        <v>0.27918258737402862</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:L5" si="1">_xlfn.STDEV.S(B2:B22)</f>
+        <v>0.10966170125175262</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>0.11506766668232402</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>0.16844788652930717</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1.04169</v>
       </c>
@@ -492,7 +547,7 @@
         <v>0.97766666666666668</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.75737999999999994</v>
       </c>
@@ -506,7 +561,7 @@
         <v>0.7436666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.79013999999999995</v>
       </c>
@@ -519,8 +574,20 @@
       <c r="D8">
         <v>0.61066666666666669</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.57368999999999992</v>
       </c>
@@ -533,8 +600,24 @@
       <c r="D9">
         <v>0.82966666666666666</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I9" s="1">
+        <f>I4/$L$4</f>
+        <v>0.96955675858568757</v>
+      </c>
+      <c r="J9" s="1">
+        <f>J4/$L$4</f>
+        <v>0.99179157502960591</v>
+      </c>
+      <c r="K9" s="1">
+        <f>K4/$L$4</f>
+        <v>1.0330942310945694</v>
+      </c>
+      <c r="L9" s="1">
+        <f>L4/$L$4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.49061999999999995</v>
       </c>
@@ -547,8 +630,24 @@
       <c r="D10">
         <v>1.1886666666666668</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I10" s="1">
+        <f>I5/$L$4</f>
+        <v>0.33061717334092378</v>
+      </c>
+      <c r="J10" s="1">
+        <f>J5/$L$4</f>
+        <v>0.12986498202711358</v>
+      </c>
+      <c r="K10" s="1">
+        <f>K5/$L$4</f>
+        <v>0.13626690353176588</v>
+      </c>
+      <c r="L10" s="1">
+        <f>L5/$L$4</f>
+        <v>0.19948151001609715</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.57602999999999982</v>
       </c>
@@ -562,7 +661,7 @@
         <v>1.0896666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1.0428599999999999</v>
       </c>
@@ -576,7 +675,7 @@
         <v>0.79666666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1.05339</v>
       </c>
@@ -590,7 +689,7 @@
         <v>0.89866666666666661</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1.5155399999999999</v>
       </c>
@@ -604,7 +703,7 @@
         <v>0.7406666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0.60060000000000002</v>
       </c>
@@ -618,7 +717,7 @@
         <v>0.84666666666666668</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0.70589999999999986</v>
       </c>

</xml_diff>